<commit_message>
added circle and graph save
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,6 +27,18 @@
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <color rgb="0000ff00"/>
+    </font>
+    <font>
+      <color rgb="00e66419"/>
+    </font>
+    <font>
+      <color rgb="00000000"/>
+    </font>
+    <font>
+      <color rgb="00ff0000"/>
     </font>
   </fonts>
   <fills count="2">
@@ -55,11 +67,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -434,13 +462,13 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Green Status: 11 projects</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr"/>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Amber Status: 1 projects</t>
         </is>
@@ -450,7 +478,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>On Hold: 1 projects</t>
         </is>
@@ -460,162 +488,129 @@
           <t xml:space="preserve">  </t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>Red Status: 0 projects</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>Project abc: 00</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="7" t="inlineStr">
         <is>
           <t>Project 123: 11</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="8" t="inlineStr">
         <is>
           <t>Project Twinkle Toes: 12</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
+      <c r="G2" s="9" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Project bcd: 01</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="C3" s="7" t="inlineStr"/>
+      <c r="E3" s="8" t="inlineStr"/>
+      <c r="G3" s="9" t="inlineStr"/>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="6" t="inlineStr">
         <is>
           <t>Project cde: 02</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-      <c r="G4" t="inlineStr"/>
+      <c r="C4" s="7" t="inlineStr"/>
+      <c r="E4" s="8" t="inlineStr"/>
+      <c r="G4" s="9" t="inlineStr"/>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="6" t="inlineStr">
         <is>
           <t>Project def: 03</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-      <c r="G5" t="inlineStr"/>
+      <c r="C5" s="7" t="inlineStr"/>
+      <c r="E5" s="8" t="inlineStr"/>
+      <c r="G5" s="9" t="inlineStr"/>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="6" t="inlineStr">
         <is>
           <t>Project efg: 04</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="C6" s="7" t="inlineStr"/>
+      <c r="E6" s="8" t="inlineStr"/>
+      <c r="G6" s="9" t="inlineStr"/>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="6" t="inlineStr">
         <is>
           <t>Project fgh: 05</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
+      <c r="C7" s="7" t="inlineStr"/>
+      <c r="E7" s="8" t="inlineStr"/>
+      <c r="G7" s="9" t="inlineStr"/>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="6" t="inlineStr">
         <is>
           <t>Project ghi: 06</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+      <c r="C8" s="7" t="inlineStr"/>
+      <c r="E8" s="8" t="inlineStr"/>
+      <c r="G8" s="9" t="inlineStr"/>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="6" t="inlineStr">
         <is>
           <t>Project hij: 07</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="C9" s="7" t="inlineStr"/>
+      <c r="E9" s="8" t="inlineStr"/>
+      <c r="G9" s="9" t="inlineStr"/>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="6" t="inlineStr">
         <is>
           <t>Project ijk: 08</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-      <c r="G10" t="inlineStr"/>
+      <c r="C10" s="7" t="inlineStr"/>
+      <c r="E10" s="8" t="inlineStr"/>
+      <c r="G10" s="9" t="inlineStr"/>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="6" t="inlineStr">
         <is>
           <t>Project jkl: 09</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-      <c r="G11" t="inlineStr"/>
+      <c r="C11" s="7" t="inlineStr"/>
+      <c r="E11" s="8" t="inlineStr"/>
+      <c r="G11" s="9" t="inlineStr"/>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="6" t="inlineStr">
         <is>
           <t>Project klm: 10</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
+      <c r="C12" s="7" t="inlineStr"/>
+      <c r="E12" s="8" t="inlineStr"/>
+      <c r="G12" s="9" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>